<commit_message>
Corrected error in excel file
</commit_message>
<xml_diff>
--- a/assignment4/job_linalg_study.xlsx
+++ b/assignment4/job_linalg_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utsacloud-my.sharepoint.com/personal/juancamilo_velasquezgonzalez_utsa_edu/Documents/PHD_Files/Clases/HPC/assignment4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2E9A68F-C9C7-49BB-A03B-9945F9A3A631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{C2E9A68F-C9C7-49BB-A03B-9945F9A3A631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{859771B3-F41A-48FA-A287-48042D613A28}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8437902-FF7E-4D08-94FA-8B2796074AE6}"/>
   </bookViews>
@@ -75,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -183,22 +183,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -208,7 +197,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -218,18 +206,7 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -324,13 +301,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -343,6 +313,25 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1890,22 +1879,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49319513058754139</c:v>
+                  <c:v>2.0275950389224322</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29288104927640612</c:v>
+                  <c:v>3.4143554267871092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18553942949486935</c:v>
+                  <c:v>5.3896899582072528</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14005732279928851</c:v>
+                  <c:v>7.1399337072369056</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13662273606295885</c:v>
+                  <c:v>7.3194259522015228</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13644143820624866</c:v>
+                  <c:v>7.3291517089432343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4413,17 +4402,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68A1E362-BB48-4543-935C-7AC6D17103B5}" name="Table1" displayName="Table1" ref="A2:E9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68A1E362-BB48-4543-935C-7AC6D17103B5}" name="Table1" displayName="Table1" ref="A2:E9" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A2:E9" xr:uid="{68A1E362-BB48-4543-935C-7AC6D17103B5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1C13E04E-8E6D-4114-9629-02CAB40638F2}" name="MKL_NUM_THREADS" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{06422001-D4BE-431E-B17F-C54D3D7494E1}" name="Creation K and F" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{34BC2DDE-D199-4FCD-A864-85042CA9C030}" name="Solution System" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{41F54C5C-1BDF-420C-9500-8ABB2B808AD8}" name="Total Time" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{1C13E04E-8E6D-4114-9629-02CAB40638F2}" name="MKL_NUM_THREADS" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{06422001-D4BE-431E-B17F-C54D3D7494E1}" name="Creation K and F" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{34BC2DDE-D199-4FCD-A864-85042CA9C030}" name="Solution System" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{41F54C5C-1BDF-420C-9500-8ABB2B808AD8}" name="Total Time" dataDxfId="1">
       <calculatedColumnFormula>B3+C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{74BA8C25-5BC0-4C06-A2FC-E51A57A99096}" name="Speed Up" dataDxfId="1">
-      <calculatedColumnFormula>D3/$D$3</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{74BA8C25-5BC0-4C06-A2FC-E51A57A99096}" name="Speed Up" dataDxfId="0">
+      <calculatedColumnFormula>$D$3/D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4730,7 +4719,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4742,13 +4731,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4782,7 +4771,7 @@
         <v>8.497954845999999</v>
       </c>
       <c r="E3" s="3">
-        <f>D3/$D$3</f>
+        <f t="shared" ref="E3:E9" si="0">$D$3/D3</f>
         <v>1</v>
       </c>
     </row>
@@ -4797,12 +4786,12 @@
         <v>4.0369338990000001</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D9" si="0">B4+C4</f>
+        <f t="shared" ref="D4:D9" si="1">B4+C4</f>
         <v>4.1911499499999998</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E9" si="1">D4/$D$3</f>
-        <v>0.49319513058754139</v>
+        <f t="shared" si="0"/>
+        <v>2.0275950389224322</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4816,12 +4805,12 @@
         <v>2.3269233699999998</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4888899319999997</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.29288104927640612</v>
+        <f t="shared" si="0"/>
+        <v>3.4143554267871092</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4835,12 +4824,12 @@
         <v>1.411990166</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5767056940000002</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.18553942949486935</v>
+        <f t="shared" si="0"/>
+        <v>5.3896899582072528</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4854,12 +4843,12 @@
         <v>1.0278263089999999</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1902008049999999</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.14005732279928851</v>
+        <f t="shared" si="0"/>
+        <v>7.1399337072369056</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4873,12 +4862,12 @@
         <v>1.000637293</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.161013842</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.13662273606295885</v>
+        <f t="shared" si="0"/>
+        <v>7.3194259522015228</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4892,12 +4881,12 @@
         <v>0.99943876300000001</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1594731810000001</v>
       </c>
-      <c r="E9" s="9">
-        <f t="shared" si="1"/>
-        <v>0.13644143820624866</v>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>7.3291517089432343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>